<commit_message>
Funções documentadas, alterado fluxo do código e adicionado ambiente
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -419,13 +419,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17.28515625" customWidth="1" min="1" max="1"/>
     <col width="22.7109375" customWidth="1" min="2" max="2"/>
@@ -4190,6 +4190,293 @@
         <v>4.629629629629629e-05</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15 /05/ 2023 17:02:55 </t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15 /05/ 2023 17:02:54 </t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>17:09:25</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>17:09:26</t>
+        </is>
+      </c>
+      <c r="E161" s="3" t="n">
+        <v>1.157407407407407e-05</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>17:09:27</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>17:09:27</t>
+        </is>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>17:09:31</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>-2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>17:09:32</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>17:09:30</t>
+        </is>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>-2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>17:09:25</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>17:09:26</t>
+        </is>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>1.157407407407407e-05</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>17:09:27</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>17:09:27</t>
+        </is>
+      </c>
+      <c r="E167" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>17:09:31</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>17:09:29</t>
+        </is>
+      </c>
+      <c r="E169" s="3" t="n">
+        <v>-2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>17:09:32</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>17:09:30</t>
+        </is>
+      </c>
+      <c r="E170" s="3" t="n">
+        <v>-2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>17:09:46</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>15 /05/ 2023</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>17:09:30</t>
+        </is>
+      </c>
+      <c r="E171" s="3" t="n">
+        <v>1.157407407407407e-05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterado Bug que não realizava aritmética com as horas.
</commit_message>
<xml_diff>
--- a/Controle de Ponto.xlsx
+++ b/Controle de Ponto.xlsx
@@ -419,13 +419,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F177"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17.28515625" customWidth="1" min="1" max="1"/>
     <col width="22.7109375" customWidth="1" min="2" max="2"/>
@@ -4627,6 +4627,156 @@
         <v>4.629629629629629e-05</v>
       </c>
     </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>18:53:26</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>18:53:28</t>
+        </is>
+      </c>
+      <c r="E178" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>18:55:06</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>18:55:08</t>
+        </is>
+      </c>
+      <c r="E179" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>18:55:06</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>18:55:08</t>
+        </is>
+      </c>
+      <c r="E180" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>18:55:06</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>18:55:08</t>
+        </is>
+      </c>
+      <c r="E181" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>18:55:15</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>18:55:15</t>
+        </is>
+      </c>
+      <c r="E182" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>18:55:48</t>
+        </is>
+      </c>
+      <c r="E183" s="3" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>